<commit_message>
turned line chart into bar chart
</commit_message>
<xml_diff>
--- a/poster/charts.xlsx
+++ b/poster/charts.xlsx
@@ -129,12 +129,14 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$A$1:$A$7</c:f>
@@ -194,7 +196,6 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -204,13 +205,12 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="618613248"/>
-        <c:axId val="133405440"/>
-      </c:lineChart>
+        <c:gapWidth val="150"/>
+        <c:axId val="99749376"/>
+        <c:axId val="60468608"/>
+      </c:barChart>
       <c:catAx>
-        <c:axId val="618613248"/>
+        <c:axId val="99749376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -219,7 +219,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133405440"/>
+        <c:crossAx val="60468608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -227,7 +227,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="133405440"/>
+        <c:axId val="60468608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="55"/>
@@ -239,7 +239,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="618613248"/>
+        <c:crossAx val="99749376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -363,11 +363,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="112252416"/>
-        <c:axId val="133400832"/>
+        <c:axId val="119755264"/>
+        <c:axId val="60470336"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="112252416"/>
+        <c:axId val="119755264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -377,7 +377,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133400832"/>
+        <c:crossAx val="60470336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -385,7 +385,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="133400832"/>
+        <c:axId val="60470336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -396,7 +396,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112252416"/>
+        <c:crossAx val="119755264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -447,16 +447,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>300037</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>147637</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>280987</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>

</xml_diff>

<commit_message>
updated the other chart to contain min, max, and avg accuracies
</commit_message>
<xml_diff>
--- a/poster/charts.xlsx
+++ b/poster/charts.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>hydrophobicity</t>
   </si>
@@ -37,6 +37,15 @@
   </si>
   <si>
     <t>NCI</t>
+  </si>
+  <si>
+    <t>Min</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>Avg</t>
   </si>
 </sst>
 </file>
@@ -206,11 +215,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="99749376"/>
-        <c:axId val="60468608"/>
+        <c:axId val="113162240"/>
+        <c:axId val="41464320"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="99749376"/>
+        <c:axId val="113162240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -219,7 +228,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="60468608"/>
+        <c:crossAx val="41464320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -227,7 +236,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="60468608"/>
+        <c:axId val="41464320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="55"/>
@@ -239,7 +248,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99749376"/>
+        <c:crossAx val="113162240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -281,7 +290,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Average classification accuracy by #</a:t>
+              <a:t>Classification accuracy by #</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
@@ -303,6 +312,17 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Min</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$A$9:$A$13</c:f>
@@ -334,16 +354,144 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>61.84</c:v>
+                  <c:v>57.03</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>69.319999999999993</c:v>
+                  <c:v>68.92</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>70.67</c:v>
+                  <c:v>70.36</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>72.069999999999993</c:v>
+                  <c:v>71.67</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>72.56</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Avg</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$9:$A$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$9:$C$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>61.841428571428573</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>69.318333333333328</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>70.668000000000006</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>72.068571428571431</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>72.56</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Max</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$9:$A$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$9:$D$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>68.08</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>69.88</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>71.48</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>72.459999999999994</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>72.56</c:v>
@@ -363,11 +511,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="119755264"/>
-        <c:axId val="60470336"/>
+        <c:axId val="113163776"/>
+        <c:axId val="41466048"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="119755264"/>
+        <c:axId val="113163776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -377,7 +525,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="60470336"/>
+        <c:crossAx val="41466048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -385,9 +533,11 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="60470336"/>
+        <c:axId val="41466048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="73"/>
+          <c:min val="57"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -396,11 +546,16 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="119755264"/>
+        <c:crossAx val="113163776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -447,16 +602,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>280987</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>185737</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>204787</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>52387</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>257175</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -765,10 +920,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -776,7 +931,7 @@
     <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -784,7 +939,7 @@
         <v>65.010000000000005</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -792,7 +947,7 @@
         <v>67.31</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -800,7 +955,7 @@
         <v>57.8</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -808,7 +963,7 @@
         <v>68.08</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -816,7 +971,7 @@
         <v>58.04</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -824,7 +979,7 @@
         <v>59.62</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -832,43 +987,205 @@
         <v>57.03</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1</v>
       </c>
       <c r="B9">
-        <v>61.84</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <f>MIN(A16:G16)</f>
+        <v>57.03</v>
+      </c>
+      <c r="C9">
+        <f>AVERAGE(A16:G16)</f>
+        <v>61.841428571428573</v>
+      </c>
+      <c r="D9">
+        <f>MAX(A16:G16)</f>
+        <v>68.08</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2</v>
       </c>
       <c r="B10">
-        <v>69.319999999999993</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+        <f>MIN(A17:G17)</f>
+        <v>68.92</v>
+      </c>
+      <c r="C10">
+        <f t="shared" ref="C10:C13" si="0">AVERAGE(A17:G17)</f>
+        <v>69.318333333333328</v>
+      </c>
+      <c r="D10">
+        <f t="shared" ref="D10:D13" si="1">MAX(A17:G17)</f>
+        <v>69.88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>3</v>
       </c>
       <c r="B11">
-        <v>70.67</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+        <f t="shared" ref="B11:B13" si="2">MIN(A18:G18)</f>
+        <v>70.36</v>
+      </c>
+      <c r="C11">
+        <f>AVERAGE(A18:G18)</f>
+        <v>70.668000000000006</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="1"/>
+        <v>71.48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>6</v>
       </c>
       <c r="B12">
-        <v>72.069999999999993</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>71.67</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>72.068571428571431</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="1"/>
+        <v>72.459999999999994</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>7</v>
       </c>
       <c r="B13">
+        <f t="shared" si="2"/>
+        <v>72.56</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>72.56</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="1"/>
+        <v>72.56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>65.010000000000005</v>
+      </c>
+      <c r="B16">
+        <v>67.31</v>
+      </c>
+      <c r="C16">
+        <v>57.8</v>
+      </c>
+      <c r="D16">
+        <v>68.08</v>
+      </c>
+      <c r="E16">
+        <v>58.04</v>
+      </c>
+      <c r="F16">
+        <v>59.62</v>
+      </c>
+      <c r="G16">
+        <v>57.03</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>69.3</v>
+      </c>
+      <c r="B17">
+        <v>68.92</v>
+      </c>
+      <c r="C17">
+        <v>68.97</v>
+      </c>
+      <c r="D17">
+        <v>69.209999999999994</v>
+      </c>
+      <c r="E17">
+        <v>69.88</v>
+      </c>
+      <c r="F17">
+        <v>69.63</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>70.569999999999993</v>
+      </c>
+      <c r="B18">
+        <v>70.39</v>
+      </c>
+      <c r="C18">
+        <v>71.48</v>
+      </c>
+      <c r="D18">
+        <v>70.540000000000006</v>
+      </c>
+      <c r="E18">
+        <v>70.36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>72.400000000000006</v>
+      </c>
+      <c r="B19">
+        <v>72.290000000000006</v>
+      </c>
+      <c r="C19">
+        <v>71.790000000000006</v>
+      </c>
+      <c r="D19">
+        <v>71.92</v>
+      </c>
+      <c r="E19">
+        <v>72.459999999999994</v>
+      </c>
+      <c r="F19">
+        <v>71.67</v>
+      </c>
+      <c r="G19">
+        <v>71.95</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>72.56</v>
+      </c>
+      <c r="B20">
+        <v>72.56</v>
+      </c>
+      <c r="C20">
+        <v>72.56</v>
+      </c>
+      <c r="D20">
+        <v>72.56</v>
+      </c>
+      <c r="E20">
+        <v>72.56</v>
+      </c>
+      <c r="F20">
+        <v>72.56</v>
+      </c>
+      <c r="G20">
         <v>72.56</v>
       </c>
     </row>

</xml_diff>